<commit_message>
Add Duckdb to scope (#1)
* add duckdb

* duckdb stats

* fix img
</commit_message>
<xml_diff>
--- a/img/results.xlsx
+++ b/img/results.xlsx
@@ -5,33 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alikefia/hacks/py-df-cmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alikefia/py-df-cmp/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F942548-7DA7-1845-939A-C19019445211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03599C1-B85D-F744-A8D7-DF1641CB3937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{A585C6B0-4AE8-3C4D-939C-630CA93EFA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$5:$F$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$5:$F$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$5</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Exec Time (s)</t>
   </si>
@@ -82,6 +66,12 @@
   </si>
   <si>
     <t>Polars / Pandas</t>
+  </si>
+  <si>
+    <t>Duckdb</t>
+  </si>
+  <si>
+    <t>Duckdb / Pandas</t>
   </si>
 </sst>
 </file>
@@ -107,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,8 +122,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,69 +158,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -227,25 +166,17 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D5C6BE-843A-6042-AD64-598F65D04E50}">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +537,7 @@
       <c r="F3" s="1">
         <v>10.28</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="4">
         <f>(D3+E3)/C3</f>
         <v>0.93068242880171959</v>
       </c>
@@ -627,8 +558,8 @@
       <c r="F4" s="1">
         <v>2.61</v>
       </c>
-      <c r="G4" s="9">
-        <f t="shared" ref="G4:G5" si="0">(D4+E4)/C4</f>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G6" si="0">(D4+E4)/C4</f>
         <v>3.5283570369077748</v>
       </c>
     </row>
@@ -648,67 +579,110 @@
       <c r="F5" s="1">
         <v>2.12</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>3.1736526946107788</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>96.31</v>
+      </c>
+      <c r="D6" s="1">
+        <v>101.53</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7.56</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>1.1551240784965215</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9">
-        <f>C4/C3</f>
-        <v>0.51320974386530538</v>
-      </c>
-      <c r="D7" s="10">
-        <f t="shared" ref="D7:F7" si="1">D4/D3</f>
-        <v>2.0535965007020196</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.063548102383054</v>
-      </c>
-      <c r="F7" s="9">
-        <f t="shared" si="1"/>
-        <v>0.25389105058365757</v>
-      </c>
-      <c r="G7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="2">
         <f>C5/C3</f>
         <v>1.4956116783091528E-2</v>
       </c>
-      <c r="D8" s="8">
-        <f t="shared" ref="D8:F8" si="2">D5/D3</f>
+      <c r="D8" s="2">
+        <f t="shared" ref="D8:F8" si="1">D5/D3</f>
         <v>4.9843395615077224E-2</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>6.0458958517210948E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.20622568093385216</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7">
+        <f>C6/C3</f>
+        <v>0.21563227655382411</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" ref="D9:F9" si="2">D6/D3</f>
+        <v>0.27413867588292473</v>
+      </c>
+      <c r="E9" s="7">
         <f t="shared" si="2"/>
-        <v>6.0458958517210948E-2</v>
-      </c>
-      <c r="F8" s="8">
+        <v>0.21447484554280671</v>
+      </c>
+      <c r="F9" s="9">
         <f t="shared" si="2"/>
-        <v>0.20622568093385216</v>
-      </c>
-      <c r="G8" s="7"/>
+        <v>0.7354085603112841</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <f>C4/C3</f>
+        <v>0.51320974386530538</v>
+      </c>
+      <c r="D10" s="4">
+        <f>D4/D3</f>
+        <v>2.0535965007020196</v>
+      </c>
+      <c r="E10" s="10">
+        <f>E4/E3</f>
+        <v>1.063548102383054</v>
+      </c>
+      <c r="F10" s="8">
+        <f>F4/F3</f>
+        <v>0.25389105058365757</v>
+      </c>
+      <c r="G10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="G8:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>